<commit_message>
tried making a results summary markdown but failed
</commit_message>
<xml_diff>
--- a/data2019/viability.xlsx
+++ b/data2019/viability.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarosenthal/Box/Competency project/competency.git/data2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D0D07D9-313C-2441-B79D-8D8EEF367E91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132E1B81-0995-A243-9925-A095BB5CABBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13780" xr2:uid="{99DE988A-4328-EE4A-9CC8-936C664C420A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24640" windowHeight="14760" activeTab="1" xr2:uid="{99DE988A-4328-EE4A-9CC8-936C664C420A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$121</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="42">
   <si>
     <t>leafID</t>
   </si>
@@ -81,9 +85,6 @@
     <t>ARME</t>
   </si>
   <si>
-    <t>no drop, probably not inoculated</t>
-  </si>
-  <si>
     <t>CEOL</t>
   </si>
   <si>
@@ -136,13 +137,37 @@
   </si>
   <si>
     <t>*note: can't confidently figure out the leaf ids for conifer assay. Might be able to mine the notes.</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Symptomatic</t>
+  </si>
+  <si>
+    <t>Asymptomatic</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>no drop, probably not inoculated. Sample omitted</t>
+  </si>
+  <si>
+    <t>Infection</t>
+  </si>
+  <si>
+    <t>Sporangia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,6 +187,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -185,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,6 +230,13 @@
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6775D0-67F4-DB4C-97E8-8335368C5E59}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -598,49 +638,49 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
+      <c r="A4">
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
+      <c r="A5">
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -737,10 +777,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -752,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -760,10 +800,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -783,16 +823,16 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -803,31 +843,28 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
+      <c r="A13">
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -924,94 +961,94 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>85</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>12</v>
+      <c r="A21">
+        <v>234</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1019,7 +1056,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1042,7 +1079,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -1065,7 +1102,7 @@
         <v>117</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1088,7 +1125,7 @@
         <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1108,94 +1145,94 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>127</v>
+        <v>299</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="4">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>128</v>
+        <v>314</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="4">
         <v>2</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>130</v>
+        <v>361</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>138</v>
+        <v>362</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1203,7 +1240,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -1226,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
@@ -1249,7 +1286,7 @@
         <v>159</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
@@ -1272,7 +1309,7 @@
         <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
@@ -1292,10 +1329,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>169</v>
+        <v>425</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>10</v>
@@ -1306,19 +1343,19 @@
       <c r="F34" s="4">
         <v>1</v>
       </c>
-      <c r="G34" s="4">
-        <v>1</v>
-      </c>
-      <c r="H34" s="4">
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>171</v>
+        <v>426</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>10</v>
@@ -1329,57 +1366,57 @@
       <c r="F35" s="4">
         <v>2</v>
       </c>
-      <c r="G35" s="4">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4">
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>183</v>
+        <v>467</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
       </c>
-      <c r="G36" s="4">
-        <v>1</v>
-      </c>
-      <c r="H36" s="4">
-        <v>0</v>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>12</v>
+      <c r="A37">
+        <v>468</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F37" s="4">
         <v>2</v>
       </c>
-      <c r="G37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s">
-        <v>12</v>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1387,7 +1424,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>14</v>
@@ -1410,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>14</v>
@@ -1433,7 +1470,7 @@
         <v>201</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>14</v>
@@ -1456,7 +1493,7 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>14</v>
@@ -1475,11 +1512,11 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>233</v>
+      <c r="B42">
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>10</v>
@@ -1491,18 +1528,18 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>234</v>
+      <c r="B43">
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>10</v>
@@ -1517,53 +1554,53 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>12</v>
+      <c r="B44">
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" t="s">
-        <v>12</v>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>12</v>
+      <c r="B45">
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F45" s="4">
         <v>2</v>
       </c>
-      <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="s">
-        <v>12</v>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1571,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>14</v>
@@ -1594,7 +1631,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>14</v>
@@ -1617,7 +1654,7 @@
         <v>265</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>14</v>
@@ -1640,7 +1677,7 @@
         <v>266</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>14</v>
@@ -1659,11 +1696,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>299</v>
-      </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>10</v>
@@ -1675,18 +1709,15 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>314</v>
-      </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>10</v>
@@ -1698,53 +1729,47 @@
         <v>2</v>
       </c>
       <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>297</v>
-      </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F52" s="4">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>303</v>
-      </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F53" s="4">
         <v>2</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -1755,7 +1780,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>14</v>
@@ -1778,7 +1803,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>14</v>
@@ -1801,7 +1826,7 @@
         <v>329</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>14</v>
@@ -1824,7 +1849,7 @@
         <v>330</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>14</v>
@@ -1843,11 +1868,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>361</v>
-      </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>10</v>
@@ -1866,11 +1888,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>362</v>
-      </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>10</v>
@@ -1882,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -1893,15 +1912,15 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="4">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60">
         <v>1</v>
       </c>
       <c r="G60" t="s">
@@ -1916,15 +1935,15 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="4">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61">
         <v>2</v>
       </c>
       <c r="G61" t="s">
@@ -1939,7 +1958,7 @@
         <v>414</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>14</v>
@@ -1962,7 +1981,7 @@
         <v>419</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>14</v>
@@ -1985,7 +2004,7 @@
         <v>393</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>14</v>
@@ -2008,7 +2027,7 @@
         <v>394</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>14</v>
@@ -2028,64 +2047,67 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>425</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="4">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66">
         <v>1</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>426</v>
+      <c r="A67" t="s">
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="4">
-        <v>2</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="H67">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>428</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="4">
+        <v>16</v>
+      </c>
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68">
         <v>1</v>
       </c>
       <c r="G68">
@@ -2096,26 +2118,26 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>430</v>
+      <c r="A69" t="s">
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F69" s="4">
-        <v>2</v>
-      </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="H69">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -2123,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>14</v>
@@ -2146,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>14</v>
@@ -2169,7 +2191,7 @@
         <v>457</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>14</v>
@@ -2192,7 +2214,7 @@
         <v>458</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>14</v>
@@ -2212,56 +2234,56 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>467</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="4">
-        <v>1</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74" s="4">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>468</v>
+        <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="4">
-        <v>2</v>
-      </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-      <c r="H75">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75" s="4">
+        <v>0</v>
+      </c>
+      <c r="H75" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>488</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>10</v>
@@ -2272,22 +2294,19 @@
       <c r="F76" s="4">
         <v>1</v>
       </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>25</v>
+      <c r="G76" s="4">
+        <v>1</v>
+      </c>
+      <c r="H76" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>497</v>
+      <c r="A77" t="s">
+        <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>10</v>
@@ -2298,11 +2317,11 @@
       <c r="F77" s="4">
         <v>2</v>
       </c>
-      <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="H77">
-        <v>1</v>
+      <c r="G77" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -2310,7 +2329,7 @@
         <v>500</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>14</v>
@@ -2328,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -2336,7 +2355,7 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>14</v>
@@ -2359,7 +2378,7 @@
         <v>499</v>
       </c>
       <c r="C80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>14</v>
@@ -2382,7 +2401,7 @@
         <v>501</v>
       </c>
       <c r="C81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>14</v>
@@ -2401,57 +2420,57 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B82">
-        <v>9</v>
+      <c r="A82" t="s">
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F82" s="4">
         <v>1</v>
       </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
+      <c r="G82" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B83">
-        <v>11</v>
+      <c r="A83" t="s">
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F83" s="4">
         <v>2</v>
       </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
+      <c r="G83" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B84">
-        <v>10</v>
+      <c r="A84">
+        <v>297</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>10</v>
@@ -2470,11 +2489,11 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B85">
-        <v>25</v>
+      <c r="A85">
+        <v>303</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>10</v>
@@ -2486,7 +2505,7 @@
         <v>2</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -2494,7 +2513,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>14</v>
@@ -2511,7 +2530,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>14</v>
@@ -2525,7 +2544,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>14</v>
@@ -2545,7 +2564,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>14</v>
@@ -2564,57 +2583,57 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B90">
-        <v>7</v>
+      <c r="A90" t="s">
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F90" s="4">
         <v>1</v>
       </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>1</v>
+      <c r="G90" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B91">
-        <v>9</v>
+      <c r="A91" t="s">
+        <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F91" s="4">
         <v>2</v>
       </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>29</v>
+      <c r="G91" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B92">
-        <v>13</v>
+      <c r="A92">
+        <v>428</v>
       </c>
       <c r="C92" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>10</v>
@@ -2633,11 +2652,11 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B93">
-        <v>15</v>
+      <c r="A93">
+        <v>430</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>10</v>
@@ -2649,7 +2668,7 @@
         <v>2</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -2657,7 +2676,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>14</v>
@@ -2671,7 +2690,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>14</v>
@@ -2688,7 +2707,7 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>14</v>
@@ -2706,12 +2725,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>14</v>
@@ -2729,238 +2748,265 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>488</v>
+      </c>
       <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="4">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>497</v>
+      </c>
+      <c r="C99" t="s">
+        <v>23</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="4">
+        <v>2</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="4">
+        <v>1</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>25</v>
+      </c>
+      <c r="C101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="4">
+        <v>2</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="4">
+        <v>1</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="4">
+        <v>2</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>13</v>
+      </c>
+      <c r="C106" t="s">
+        <v>27</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="4">
+        <v>1</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>27</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="4">
+        <v>2</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="4">
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" s="4">
-        <v>1</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>30</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F99" s="4">
-        <v>2</v>
-      </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99" s="4" t="s">
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
-        <v>30</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="4">
-        <v>1</v>
-      </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100" s="4" t="s">
+      <c r="D109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" s="4">
+        <v>2</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C101" t="s">
-        <v>30</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F101" s="4">
-        <v>2</v>
-      </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C102" t="s">
-        <v>30</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
-        <v>30</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F103" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B104">
-        <v>1</v>
-      </c>
-      <c r="C104" t="s">
-        <v>30</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F104" s="4">
-        <v>1</v>
-      </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B105">
-        <v>2</v>
-      </c>
-      <c r="C105" t="s">
-        <v>30</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="4">
-        <v>2</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C106" t="s">
-        <v>32</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E106" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" s="4">
-        <v>1</v>
-      </c>
-      <c r="G106">
-        <v>1</v>
-      </c>
-      <c r="H106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C107" t="s">
-        <v>32</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F107" s="4">
-        <v>2</v>
-      </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C108" t="s">
-        <v>32</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="4">
-        <v>1</v>
-      </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C109" t="s">
-        <v>32</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F109" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
-        <v>32</v>
-      </c>
       <c r="D110" s="4" t="s">
         <v>14</v>
       </c>
@@ -2971,9 +3017,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>14</v>
@@ -2985,9 +3031,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>14</v>
@@ -3007,7 +3053,7 @@
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>14</v>
@@ -3027,47 +3073,41 @@
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F114" s="4">
         <v>1</v>
       </c>
       <c r="G114">
-        <v>1</v>
-      </c>
-      <c r="H114">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H114" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F115" s="4">
         <v>2</v>
-      </c>
-      <c r="G115">
-        <v>1</v>
-      </c>
-      <c r="H115">
-        <v>1</v>
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>10</v>
@@ -3081,7 +3121,7 @@
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>10</v>
@@ -3095,7 +3135,7 @@
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>14</v>
@@ -3115,7 +3155,7 @@
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>14</v>
@@ -3129,7 +3169,7 @@
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>14</v>
@@ -3149,7 +3189,7 @@
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>14</v>
@@ -3170,4 +3210,309 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048552A4-D6EF-F04D-888A-BF44C501180D}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A18">
+    <sortCondition ref="A3"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>